<commit_message>
new file to R1
</commit_message>
<xml_diff>
--- a/File2/sample.xlsx
+++ b/File2/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trainings\Projects\Trident\Prj02\File2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA2028-48DB-4ECC-84A7-B670DC09696C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421A5EC6-9598-4314-81EC-CABF5A63A220}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>